<commit_message>
added results for 60.txt dataset
</commit_message>
<xml_diff>
--- a/itmd-521/Week-12/images/Graphs.xlsx
+++ b/itmd-521/Week-12/images/Graphs.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD69E7F9-D5CE-4050-91CF-B83633D080E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A249C1-CD15-41F2-8ECF-B7152753DE46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part2" sheetId="1" r:id="rId1"/>
     <sheet name="Part3" sheetId="2" r:id="rId2"/>
+    <sheet name="Part3-2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>One Reducer</t>
   </si>
@@ -791,6 +792,186 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-DABC-4FB9-A296-EE8CD4B0BC7C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-DABC-4FB9-A296-EE8CD4B0BC7C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-DABC-4FB9-A296-EE8CD4B0BC7C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001C-DABC-4FB9-A296-EE8CD4B0BC7C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-DABC-4FB9-A296-EE8CD4B0BC7C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-DABC-4FB9-A296-EE8CD4B0BC7C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-DABC-4FB9-A296-EE8CD4B0BC7C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Part3!$A$1:$H$1</c:f>
@@ -835,11 +1016,23 @@
                 <c:pt idx="1">
                   <c:v>157</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>304</c:v>
+                </c:pt>
                 <c:pt idx="4">
-                  <c:v>34</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34</c:v>
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="#,##0">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0">
+                  <c:v>549</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1121,6 +1314,656 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing execution time (Seconds) for running the job with</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>combiner and without combiner</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> considering the number of reducers</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F72F-4324-A463-CB5E1E54D382}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F72F-4324-A463-CB5E1E54D382}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F72F-4324-A463-CB5E1E54D382}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F72F-4324-A463-CB5E1E54D382}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-F72F-4324-A463-CB5E1E54D382}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-F72F-4324-A463-CB5E1E54D382}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-F72F-4324-A463-CB5E1E54D382}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Part3-2'!$A$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1 Reducer</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Reducers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4 Reducers</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 Reducers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1 Reducer / Combiner</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2 Reducer / Combiner</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4 Reducer / Combiner</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8 Reducer / Combiner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Part3-2'!$A$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3189</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3137</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4544</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-F72F-4324-A463-CB5E1E54D382}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="95"/>
+        <c:overlap val="100"/>
+        <c:axId val="583431048"/>
+        <c:axId val="583431376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="583431048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="583431376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="583431376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="583431048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1201,6 +2044,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="304">
   <cs:axisTitle>
@@ -1698,6 +2581,502 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="304">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="304">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2255,6 +3634,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4446F9F8-8E4B-4CFD-BC16-C2DCE2814E56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1" descr="sdf" title="dfs">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F2E11BB-FBB0-4B13-B65D-07AB821535B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2598,8 +4020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFF073F-5284-4616-A731-A70D561BA367}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2645,11 +4067,81 @@
       <c r="B2">
         <v>157</v>
       </c>
+      <c r="C2">
+        <v>121</v>
+      </c>
+      <c r="D2">
+        <v>304</v>
+      </c>
       <c r="E2">
-        <v>34</v>
+        <v>190</v>
       </c>
       <c r="F2">
-        <v>34</v>
+        <v>236</v>
+      </c>
+      <c r="G2" s="1">
+        <v>258</v>
+      </c>
+      <c r="H2" s="1">
+        <v>549</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532E8B13-6885-4EBB-92D7-0992AA49005F}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3189</v>
+      </c>
+      <c r="B2">
+        <v>3137</v>
+      </c>
+      <c r="C2">
+        <v>4544</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>

</xml_diff>

<commit_message>
Add more result for 60-90.txt
</commit_message>
<xml_diff>
--- a/itmd-521/Week-12/images/Graphs.xlsx
+++ b/itmd-521/Week-12/images/Graphs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3251649B-19AE-49F7-8FA2-AB7CF268CFF1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67C6CDC-8E26-4378-B89C-BC3FD869EE95}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part2" sheetId="1" r:id="rId1"/>
@@ -1687,6 +1687,12 @@
                 <c:pt idx="3">
                   <c:v>2358</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>8558</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3522</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3671,8 +3677,8 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4023,7 +4029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFF073F-5284-4616-A731-A70D561BA367}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -4099,8 +4105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532E8B13-6885-4EBB-92D7-0992AA49005F}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4149,6 +4155,12 @@
       <c r="D2">
         <v>2358</v>
       </c>
+      <c r="E2">
+        <v>8558</v>
+      </c>
+      <c r="F2">
+        <v>3522</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>

</xml_diff>

<commit_message>
edit README file for part 2
</commit_message>
<xml_diff>
--- a/itmd-521/Week-12/images/Graphs.xlsx
+++ b/itmd-521/Week-12/images/Graphs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1116E623-DEE7-4839-A90A-C665D42BF8CC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D16A507-B186-416E-8D00-ACA5B0D66856}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part2" sheetId="1" r:id="rId1"/>
@@ -3979,7 +3979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFF073F-5284-4616-A731-A70D561BA367}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -4053,10 +4053,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532E8B13-6885-4EBB-92D7-0992AA49005F}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4118,6 +4118,11 @@
         <v>14688</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>4283</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>